<commit_message>
Att lista de cameras
</commit_message>
<xml_diff>
--- a/src/assets/Cameras.xlsx
+++ b/src/assets/Cameras.xlsx
@@ -982,7 +982,7 @@
     <t xml:space="preserve">PSJC-CSI-643.2</t>
   </si>
   <si>
-    <t xml:space="preserve">PSJC-CSI.643.1</t>
+    <t xml:space="preserve">PSJC-CSI-643.1</t>
   </si>
   <si>
     <t xml:space="preserve">PSJC-CSI-642.2</t>
@@ -3779,8 +3779,8 @@
   </sheetPr>
   <dimension ref="A1:A1215"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:1215"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A301" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F325" activeCellId="0" sqref="F325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>